<commit_message>
Created Product And Customers
</commit_message>
<xml_diff>
--- a/AddOn_TestData.xlsx
+++ b/AddOn_TestData.xlsx
@@ -5,20 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCurrency" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="AddProductCategory1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="AddProductCategory" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CreateOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>admin</t>
   </si>
@@ -29,18 +28,33 @@
     <t>Sanity Suite Test</t>
   </si>
   <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>SMS Local</t>
+  </si>
+  <si>
+    <t>SMSLCL</t>
+  </si>
+  <si>
+    <t>'01/01/2018'</t>
+  </si>
+  <si>
+    <t>SMSBundle</t>
+  </si>
+  <si>
+    <t>SMSBundle100</t>
+  </si>
+  <si>
+    <t>SMS100</t>
+  </si>
+  <si>
+    <t>Test Category</t>
+  </si>
+  <si>
     <t>Sanity Suite Test Child</t>
   </si>
   <si>
-    <t>Currencies updated successfully.</t>
-  </si>
-  <si>
-    <t>Working as admin Sanity Suite Test Child X</t>
-  </si>
-  <si>
-    <t>Test Category</t>
-  </si>
-  <si>
     <t>Test Product1</t>
   </si>
   <si>
@@ -77,16 +91,13 @@
     <t>Default</t>
   </si>
   <si>
-    <t>USD Customer</t>
-  </si>
-  <si>
-    <t>CAD Customer</t>
-  </si>
-  <si>
-    <t>Euro Customer</t>
-  </si>
-  <si>
-    <t>'01/26/2017'</t>
+    <t>AddOnCustomer1</t>
+  </si>
+  <si>
+    <t>AddOnCustomer2</t>
+  </si>
+  <si>
+    <t>AddOnCustomer3</t>
   </si>
 </sst>
 </file>
@@ -171,25 +182,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -209,52 +216,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1:C2 F1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="F:F D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.03703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.02962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.3037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.84814814814815"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.94074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.3037037037037"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.94074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -266,8 +314,8 @@
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="C1:C2 G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="F:F G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -288,26 +336,26 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>10</v>
@@ -324,17 +372,17 @@
       <c r="M1" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="R1" s="3"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>11</v>
@@ -354,13 +402,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>12</v>
@@ -380,13 +428,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>13</v>
@@ -405,11 +453,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>14</v>
@@ -428,11 +476,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="3" t="s">
-        <v>16</v>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>15</v>
@@ -451,11 +499,11 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>9</v>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>16</v>
@@ -474,11 +522,11 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="3" t="s">
-        <v>17</v>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>17</v>
@@ -497,11 +545,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="3" t="s">
-        <v>17</v>
+      <c r="G9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>18</v>
@@ -540,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1:C2 E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +598,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9296296296296"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.97777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8592592592593"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8851851851852"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
   </cols>
@@ -566,205 +614,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="1" sqref="C1:C2 E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.02962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.3037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.84814814814815"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.94074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.3037037037037"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.94074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36296296296296"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="n">
-        <v>90</v>
-      </c>
-      <c r="I1" s="4" t="n">
-        <v>120</v>
-      </c>
-      <c r="J1" s="4" t="n">
-        <v>93</v>
-      </c>
-      <c r="K1" s="4" t="n">
-        <v>123</v>
-      </c>
-      <c r="L1" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="M1" s="4" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>90</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>120</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>93</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>123</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>99</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>129</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>102</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>132</v>
-      </c>
-      <c r="L3" s="4" t="n">
-        <v>105</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>108</v>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>138</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>111</v>
-      </c>
-      <c r="K4" s="4" t="n">
-        <v>141</v>
-      </c>
-      <c r="L4" s="4" t="n">
-        <v>114</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>144</v>
-      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added the 2 Test Cases of the AddOn
</commit_message>
<xml_diff>
--- a/AddOn_TestData.xlsx
+++ b/AddOn_TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="AddProductCategory" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AddOrder" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>admin</t>
   </si>
@@ -25,7 +25,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Sanity Suite Test</t>
+    <t>Web Data Technologies</t>
   </si>
   <si>
     <t>SMS</t>
@@ -49,55 +49,37 @@
     <t>SMS100</t>
   </si>
   <si>
-    <t>Test Category</t>
-  </si>
-  <si>
-    <t>Sanity Suite Test Child</t>
-  </si>
-  <si>
-    <t>Test Product1</t>
-  </si>
-  <si>
-    <t>'01/01/1970'</t>
-  </si>
-  <si>
-    <t>United States Dollar</t>
-  </si>
-  <si>
-    <t>Test Product2</t>
-  </si>
-  <si>
-    <t>Canadian Dollar</t>
-  </si>
-  <si>
-    <t>Test Product3</t>
-  </si>
-  <si>
-    <t>Euro</t>
-  </si>
-  <si>
-    <t>Test Product4</t>
-  </si>
-  <si>
-    <t>'06/26/2018'</t>
-  </si>
-  <si>
-    <t>06/26/2018</t>
-  </si>
-  <si>
-    <t>'01/01/2020'</t>
+    <t>AddOnCustomer1</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>pre paid</t>
+  </si>
+  <si>
+    <t>'01/31/2018'</t>
+  </si>
+  <si>
+    <t>Total = US$0.00</t>
+  </si>
+  <si>
+    <t>AddOnCustomer2</t>
+  </si>
+  <si>
+    <t>'01/15/2018'</t>
+  </si>
+  <si>
+    <t>AddOnCustomer3</t>
+  </si>
+  <si>
+    <t>'01/17/2018'</t>
+  </si>
+  <si>
+    <t>Total = US$5.00</t>
   </si>
   <si>
     <t>Default</t>
-  </si>
-  <si>
-    <t>AddOnCustomer1</t>
-  </si>
-  <si>
-    <t>AddOnCustomer2</t>
-  </si>
-  <si>
-    <t>AddOnCustomer3</t>
   </si>
 </sst>
 </file>
@@ -182,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +178,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,14 +205,14 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="F:F D10"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0703703703704"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3148148148148"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1555555555556"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6333333333333"/>
@@ -261,7 +247,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>0.25</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -273,7 +259,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
@@ -283,8 +269,8 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>10</v>
+      <c r="G2" s="1" t="n">
+        <v>0.25</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -312,10 +298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="F:F G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -323,16 +309,20 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96296296296296"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.70740740740741"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.85555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.67037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.88518518518518"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.85555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -342,228 +332,138 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>10</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="K1" s="0" t="n">
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="L1" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>31</v>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="M2" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>51</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>12</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="M3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="M4" s="0" t="n">
+      <c r="N4" s="0" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="M5" s="0" t="n">
+      <c r="F5" s="2"/>
+      <c r="N5" s="0" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="M6" s="0" t="n">
+      <c r="F6" s="2"/>
+      <c r="N6" s="0" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="M7" s="0" t="n">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="N7" s="0" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="M8" s="0" t="n">
+      <c r="F8" s="2"/>
+      <c r="N8" s="0" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="M9" s="0" t="n">
+      <c r="F9" s="2"/>
+      <c r="N9" s="0" t="n">
         <v>58</v>
       </c>
     </row>
@@ -588,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -614,22 +514,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Complete automation code of Add on feature
</commit_message>
<xml_diff>
--- a/AddOn_TestData.xlsx
+++ b/AddOn_TestData.xlsx
@@ -9,15 +9,15 @@
   </bookViews>
   <sheets>
     <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="AddOrder" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AddCustomer" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="AddCustomer" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AddOrder" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>admin</t>
   </si>
@@ -25,7 +25,7 @@
     <t>WebData@123</t>
   </si>
   <si>
-    <t>Web Data Technologies</t>
+    <t>AddOn Test Suite</t>
   </si>
   <si>
     <t>SMS</t>
@@ -49,9 +49,18 @@
     <t>SMS100</t>
   </si>
   <si>
+    <t>Default</t>
+  </si>
+  <si>
     <t>AddOnCustomer1</t>
   </si>
   <si>
+    <t>AddOnCustomer2</t>
+  </si>
+  <si>
+    <t>AddOnCustomer3</t>
+  </si>
+  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -64,22 +73,28 @@
     <t>Total = US$0.00</t>
   </si>
   <si>
-    <t>AddOnCustomer2</t>
+    <t>'01/10/2018'</t>
   </si>
   <si>
     <t>'01/15/2018'</t>
   </si>
   <si>
-    <t>AddOnCustomer3</t>
+    <t>'01/11/2018'</t>
+  </si>
+  <si>
+    <t>'01/20/2018'</t>
+  </si>
+  <si>
+    <t>'01/12/2018'</t>
+  </si>
+  <si>
+    <t>Total = US$12.50</t>
   </si>
   <si>
     <t>'01/17/2018'</t>
   </si>
   <si>
     <t>Total = US$5.00</t>
-  </si>
-  <si>
-    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -204,8 +219,8 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -298,174 +313,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.70740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.67037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.88518518518518"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3925925925926"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.85555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0185185185185"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.97777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="S1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="2"/>
-      <c r="N5" s="0" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="2"/>
-      <c r="N6" s="0" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="N7" s="0" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="2"/>
-      <c r="N8" s="0" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="2"/>
-      <c r="N9" s="0" t="n">
-        <v>58</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -486,52 +379,167 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.97777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.70740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.67037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.88518518518518"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.85555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.37777777777778"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0185185185185"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4592592592593"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.1185185185185"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5703703703704"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.97037037037037"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1"/>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="L2" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
some changes in code for add on feature test plan
</commit_message>
<xml_diff>
--- a/AddOn_TestData.xlsx
+++ b/AddOn_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,88 +13,93 @@
     <sheet name="AddOrder" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>WebData@123</t>
-  </si>
-  <si>
-    <t>AddOn Test Suite</t>
-  </si>
-  <si>
-    <t>SMS</t>
-  </si>
-  <si>
-    <t>SMS Local</t>
-  </si>
-  <si>
-    <t>SMSLCL</t>
-  </si>
-  <si>
-    <t>'01/01/2018'</t>
-  </si>
-  <si>
-    <t>SMSBundle</t>
-  </si>
-  <si>
-    <t>SMSBundle100</t>
-  </si>
-  <si>
-    <t>SMS100</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>AddOnCustomer1</t>
-  </si>
-  <si>
-    <t>AddOnCustomer2</t>
-  </si>
-  <si>
-    <t>AddOnCustomer3</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>pre paid</t>
-  </si>
-  <si>
-    <t>'01/31/2018'</t>
-  </si>
-  <si>
-    <t>Total = US$0.00</t>
-  </si>
-  <si>
-    <t>'01/10/2018'</t>
-  </si>
-  <si>
-    <t>'01/15/2018'</t>
-  </si>
-  <si>
-    <t>'01/11/2018'</t>
-  </si>
-  <si>
-    <t>'01/20/2018'</t>
-  </si>
-  <si>
-    <t>'01/12/2018'</t>
-  </si>
-  <si>
-    <t>Total = US$12.50</t>
-  </si>
-  <si>
-    <t>'01/17/2018'</t>
-  </si>
-  <si>
-    <t>Total = US$5.00</t>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebData@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMS Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMSLCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/01/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMSBundle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMSBundle100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMS100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddOnCustomer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddOnCustomer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddOnCustomer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/31/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/10/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/15/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/11/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/20/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/12/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$12.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'01/17/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = US$5.00</t>
   </si>
 </sst>
 </file>
@@ -102,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
@@ -225,24 +230,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.03703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.02962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.3037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.84814814814815"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.94074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.3037037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.94074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.29259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.01851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.60740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.82222222222222"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.91851851851852"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.60740740740741"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.91851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -262,7 +267,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>10</v>
+        <v>0.25</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -274,7 +279,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
@@ -285,7 +290,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.25</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -315,19 +320,18 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.97777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,31 +385,30 @@
   </sheetPr>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.70740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.67037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.88518518518518"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3925925925926"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.85555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0185185185185"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.37777777777778"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0185185185185"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4592592592593"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.1185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5703703703704"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.97037037037037"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.19259259259259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added Filter for Customer in Product Historical Package
</commit_message>
<xml_diff>
--- a/AddOn_TestData.xlsx
+++ b/AddOn_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 67</t>
+    <t xml:space="preserve">Web Data 49</t>
   </si>
   <si>
     <t xml:space="preserve">SMS</t>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">'01/01/2018'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
     <t xml:space="preserve">SMSBundle</t>
@@ -224,30 +227,30 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.60740740740741"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="4.60740740740741"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.81851851851852"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="3.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.82"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -272,7 +275,9 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -281,13 +286,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>10</v>
@@ -305,7 +310,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -320,18 +325,18 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="C1 F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,22 +350,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -370,7 +377,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -385,30 +392,30 @@
   </sheetPr>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.19259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.81851851851852"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -422,40 +429,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>20</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L1" s="0" t="n">
         <v>25</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>6</v>
@@ -464,72 +471,72 @@
         <v>50</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2"/>
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>35</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="0" t="n">
         <v>150</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="0" t="n">
         <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>20</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R3" s="4"/>
     </row>
@@ -541,7 +548,7 @@
         <v>45</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +557,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>